<commit_message>
fixing call back file in use
</commit_message>
<xml_diff>
--- a/tests/output/data.xlsx
+++ b/tests/output/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,24 +424,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>filename</t>
+          <t>##name##</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ABC</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>test</t>
+          <t>John</t>
         </is>
       </c>
     </row>

</xml_diff>